<commit_message>
Deploying to gh-pages from  @ b65dcd9e69d767ab1abe4ffe59ffd04c695436f9 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.1.1.xlsx
+++ b/en/downloads/data-excel/10.1.1.xlsx
@@ -206,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -248,6 +248,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -554,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +578,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -580,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -591,8 +600,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
@@ -623,8 +632,11 @@
       <c r="J4" s="15">
         <v>2021</v>
       </c>
+      <c r="K4" s="16">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -655,8 +667,11 @@
       <c r="J5" s="7">
         <v>4.6024666695867751</v>
       </c>
+      <c r="K5" s="17">
+        <v>3.9462868231169921</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
@@ -686,6 +701,9 @@
       </c>
       <c r="J6" s="11">
         <v>4.3694509108608912</v>
+      </c>
+      <c r="K6" s="18">
+        <v>3.8007658934388928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ a81168b25673a30335d3c4699643d0e12a352c98 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.1.1.xlsx
+++ b/en/downloads/data-excel/10.1.1.xlsx
@@ -206,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -248,15 +248,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -563,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,7 +569,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="2" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -589,7 +580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -600,8 +591,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
@@ -632,11 +623,8 @@
       <c r="J4" s="15">
         <v>2021</v>
       </c>
-      <c r="K4" s="16">
-        <v>2022</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -667,11 +655,8 @@
       <c r="J5" s="7">
         <v>4.6024666695867751</v>
       </c>
-      <c r="K5" s="17">
-        <v>3.9462868231169921</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
@@ -701,9 +686,6 @@
       </c>
       <c r="J6" s="11">
         <v>4.3694509108608912</v>
-      </c>
-      <c r="K6" s="18">
-        <v>3.8007658934388928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 38d09626c9e296e929f3f517b58975ce4da03170 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.1.1.xlsx
+++ b/en/downloads/data-excel/10.1.1.xlsx
@@ -206,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -248,6 +248,15 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -554,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +578,7 @@
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>12</v>
       </c>
@@ -580,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -591,8 +600,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
@@ -623,8 +632,11 @@
       <c r="J4" s="15">
         <v>2021</v>
       </c>
+      <c r="K4" s="16">
+        <v>2022</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -655,8 +667,11 @@
       <c r="J5" s="7">
         <v>4.6024666695867751</v>
       </c>
+      <c r="K5" s="17">
+        <v>3.9462868231169921</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
@@ -686,6 +701,9 @@
       </c>
       <c r="J6" s="11">
         <v>4.3694509108608912</v>
+      </c>
+      <c r="K6" s="18">
+        <v>3.8007658934388928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 7530e39daa40fb3ebf07b9b79a936bf811acf424 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.1.1.xlsx
+++ b/en/downloads/data-excel/10.1.1.xlsx
@@ -31,12 +31,6 @@
     <t>The growth rate of disposable among the incom within the whole population</t>
   </si>
   <si>
-    <t>(процент)</t>
-  </si>
-  <si>
-    <t>(percent)</t>
-  </si>
-  <si>
     <t>10.1.1 Темпы роста доходов домохозяйств  на душу населения среди наименее обеспеченных 40 процентов населения и среди населения в целом</t>
   </si>
   <si>
@@ -59,6 +53,12 @@
   </si>
   <si>
     <t>(пайыз менен)</t>
+  </si>
+  <si>
+    <t>(в процентах)</t>
+  </si>
+  <si>
+    <t>(in percent)</t>
   </si>
 </sst>
 </file>
@@ -206,7 +206,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -238,19 +238,25 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -557,85 +563,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" style="1" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
+    <col min="1" max="3" width="41" style="1" customWidth="1"/>
     <col min="4" max="10" width="9.42578125" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6" t="s">
+    <row r="3" spans="1:12" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="17">
+        <v>2015</v>
+      </c>
+      <c r="E4" s="17">
+        <v>2016</v>
+      </c>
+      <c r="F4" s="17">
+        <v>2017</v>
+      </c>
+      <c r="G4" s="17">
+        <v>2018</v>
+      </c>
+      <c r="H4" s="17">
+        <v>2019</v>
+      </c>
+      <c r="I4" s="17">
+        <v>2020</v>
+      </c>
+      <c r="J4" s="17">
+        <v>2021</v>
+      </c>
+      <c r="K4" s="18">
+        <v>2022</v>
+      </c>
+      <c r="L4" s="18">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="36" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="15">
-        <v>2015</v>
-      </c>
-      <c r="E4" s="15">
-        <v>2016</v>
-      </c>
-      <c r="F4" s="15">
-        <v>2017</v>
-      </c>
-      <c r="G4" s="15">
-        <v>2018</v>
-      </c>
-      <c r="H4" s="15">
-        <v>2019</v>
-      </c>
-      <c r="I4" s="15">
-        <v>2020</v>
-      </c>
-      <c r="J4" s="15">
-        <v>2021</v>
-      </c>
-      <c r="K4" s="16">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="36" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>3</v>
@@ -664,13 +697,16 @@
       <c r="K5" s="7">
         <v>3.9462868231169921</v>
       </c>
+      <c r="L5" s="7">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>4</v>
@@ -698,6 +734,9 @@
       </c>
       <c r="K6" s="11">
         <v>3.8007658934388928</v>
+      </c>
+      <c r="L6" s="11">
+        <v>4.5999999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>